<commit_message>
Added Traffic to Scenario
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bking\Documents\Uni\Research\Thesis\Matlab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE00D411-B207-4B11-9688-D6104A418F37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{280E92B9-E038-4934-870B-036839CF6DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2490" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{BD3CB24B-432F-404A-A98A-D93107AC1766}"/>
+    <workbookView xWindow="28680" yWindow="-2490" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{BD3CB24B-432F-404A-A98A-D93107AC1766}"/>
   </bookViews>
   <sheets>
     <sheet name="PPO" sheetId="2" r:id="rId1"/>
     <sheet name="DQN" sheetId="1" r:id="rId2"/>
     <sheet name="DQN Variable Lights" sheetId="3" r:id="rId3"/>
     <sheet name="DQN Variable Lights 2" sheetId="4" r:id="rId4"/>
+    <sheet name="DQN with Traffic" sheetId="6" r:id="rId5"/>
+    <sheet name="Total_Fuel_Consumption_traffic" sheetId="5" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">PPO!$O$18:$O$67</definedName>
@@ -27,6 +29,8 @@
     <definedName name="_xlchart.v1.5" hidden="1">'DQN Variable Lights'!$S$18:$S$45</definedName>
     <definedName name="_xlchart.v1.6" hidden="1">'DQN Variable Lights 2'!$O$18:$O$67</definedName>
     <definedName name="_xlchart.v1.7" hidden="1">'DQN Variable Lights 2'!$S$18:$S$45</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">'DQN with Traffic'!$O$18:$O$67</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">'DQN with Traffic'!$S$18:$S$44</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="13">
   <si>
     <t>Training Plot</t>
   </si>
@@ -241,7 +245,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -262,6 +266,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -876,6 +881,155 @@
 </cx:chartSpace>
 </file>
 
+<file path=xl/charts/chartEx5.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.9</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="1">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.8</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{978A6524-3714-40CD-8CDB-D1B67E0D9BCA}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f/>
+              <cx:v>Baseline</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </cx:spPr>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="1" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{00000001-AE42-4F26-947C-82ED0E8C7832}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f/>
+              <cx:v>RL</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </cx:spPr>
+          <cx:dataId val="1"/>
+          <cx:layoutPr>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="1"/>
+        <cx:title>
+          <cx:txPr>
+            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+              </a:endParaRPr>
+            </a:p>
+          </cx:txPr>
+        </cx:title>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:title>
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Fuel Consumption</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:txPr>
+            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr sz="2000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="2000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+                </a:rPr>
+                <a:t>Fuel Consumption</a:t>
+              </a:r>
+            </a:p>
+          </cx:txPr>
+        </cx:title>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+    <cx:legend pos="t" align="ctr" overlay="0">
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1600"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US" sz="1600" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:sysClr>
+            </a:solidFill>
+            <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+          </a:endParaRPr>
+        </a:p>
+      </cx:txPr>
+    </cx:legend>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1036,6 +1190,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
   <cs:axisTitle>
@@ -2582,6 +2776,521 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4018,6 +4727,238 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>15387</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>95335</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{776FE6F2-C7C1-4C26-BBB5-D2B53C504F3D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1360170" y="5444490"/>
+          <a:ext cx="1707027" cy="981160"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>555172</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>398417</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="3" name="Chart 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07215DFE-24D6-4E61-9E6A-D8D90F1B6E5B}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="16896262" y="8839201"/>
+              <a:ext cx="7166065" cy="4825364"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>466454</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>33369</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>190501</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>131490</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{659E1764-1584-2A23-448E-E217014E5FEF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1691097" y="564048"/>
+          <a:ext cx="4010297" cy="3114824"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>598715</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>149679</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>434069</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>125187</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5693244F-73CB-A00E-C9A5-4126A5F39970}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1211036" y="6871608"/>
+          <a:ext cx="5346247" cy="3867150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -7651,7 +8592,7 @@
         <v>50.453516340671598</v>
       </c>
       <c r="O19" s="10">
-        <f t="shared" ref="O19:O47" si="0">N19-N$2</f>
+        <f t="shared" ref="O19:O44" si="0">N19-N$2</f>
         <v>-5.8718356011141211</v>
       </c>
       <c r="P19" s="10"/>
@@ -9161,7 +10102,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCF1E85D-9F90-4480-88ED-AA158FB4457A}">
   <dimension ref="C2:AH79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
@@ -9416,7 +10357,7 @@
         <v>54.163952916756102</v>
       </c>
       <c r="O19" s="10">
-        <f t="shared" ref="O19:O48" si="0">N19-N$2</f>
+        <f t="shared" ref="O19:O47" si="0">N19-N$2</f>
         <v>-2.1613990250296169</v>
       </c>
       <c r="P19" s="10"/>
@@ -10935,4 +11876,1958 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF394BB9-BA36-455C-B4B1-369A61AE2048}">
+  <dimension ref="C2:AH79"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="13" max="13" width="11.21875" customWidth="1"/>
+    <col min="14" max="14" width="36.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.77734375" customWidth="1"/>
+    <col min="18" max="18" width="41.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="M2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" s="12">
+        <f>AVERAGE(R18:R45)</f>
+        <v>58.597565183539118</v>
+      </c>
+    </row>
+    <row r="3" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="M3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N3" s="12">
+        <f>AVERAGE(N18:N47)</f>
+        <v>57.193274131907309</v>
+      </c>
+    </row>
+    <row r="4" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="N4" s="12"/>
+    </row>
+    <row r="5" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="M5" t="s">
+        <v>9</v>
+      </c>
+      <c r="N5" s="13">
+        <f>(N3-N2)/N2</f>
+        <v>-2.3965006860494846E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="9"/>
+      <c r="S16" s="4"/>
+    </row>
+    <row r="17" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="O17" s="10"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="10"/>
+      <c r="R17" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="S17" s="6"/>
+    </row>
+    <row r="18" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="M18" s="5"/>
+      <c r="N18">
+        <v>62.024269628153498</v>
+      </c>
+      <c r="O18" s="10">
+        <f>N18-N$2</f>
+        <v>3.42670444461438</v>
+      </c>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="10"/>
+      <c r="R18" s="16">
+        <v>63.861532910081301</v>
+      </c>
+      <c r="S18" s="6">
+        <f>R18-N$2</f>
+        <v>5.2639677265421838</v>
+      </c>
+    </row>
+    <row r="19" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="M19" s="5"/>
+      <c r="N19">
+        <v>57.420475827959599</v>
+      </c>
+      <c r="O19" s="10">
+        <f t="shared" ref="O19:O47" si="0">N19-N$2</f>
+        <v>-1.1770893555795183</v>
+      </c>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="10"/>
+      <c r="R19" s="16">
+        <v>70.607795284247501</v>
+      </c>
+      <c r="S19" s="6">
+        <f t="shared" ref="S19:S47" si="1">R19-N$2</f>
+        <v>12.010230100708384</v>
+      </c>
+    </row>
+    <row r="20" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="M20" s="5"/>
+      <c r="N20">
+        <v>51.574472556961801</v>
+      </c>
+      <c r="O20" s="10">
+        <f t="shared" si="0"/>
+        <v>-7.0230926265773164</v>
+      </c>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="16">
+        <v>50.838459080163098</v>
+      </c>
+      <c r="S20" s="6">
+        <f t="shared" si="1"/>
+        <v>-7.7591061033760198</v>
+      </c>
+    </row>
+    <row r="21" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="M21" s="5"/>
+      <c r="N21">
+        <v>52.171653121815801</v>
+      </c>
+      <c r="O21" s="10">
+        <f t="shared" si="0"/>
+        <v>-6.4259120617233165</v>
+      </c>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="16">
+        <v>64.319927451827198</v>
+      </c>
+      <c r="S21" s="6">
+        <f t="shared" si="1"/>
+        <v>5.7223622682880801</v>
+      </c>
+    </row>
+    <row r="22" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="M22" s="5"/>
+      <c r="N22">
+        <v>57.082714594657503</v>
+      </c>
+      <c r="O22" s="10">
+        <f t="shared" si="0"/>
+        <v>-1.5148505888816146</v>
+      </c>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="10"/>
+      <c r="R22" s="16">
+        <v>54.376935072882503</v>
+      </c>
+      <c r="S22" s="6">
+        <f t="shared" si="1"/>
+        <v>-4.2206301106566144</v>
+      </c>
+    </row>
+    <row r="23" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="M23" s="5"/>
+      <c r="N23">
+        <v>63.619323385905503</v>
+      </c>
+      <c r="O23" s="10">
+        <f t="shared" si="0"/>
+        <v>5.0217582023663851</v>
+      </c>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="10"/>
+      <c r="R23" s="16">
+        <v>48.3059581991551</v>
+      </c>
+      <c r="S23" s="6">
+        <f t="shared" si="1"/>
+        <v>-10.291606984384018</v>
+      </c>
+    </row>
+    <row r="24" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="M24" s="5"/>
+      <c r="N24">
+        <v>53.500400414071301</v>
+      </c>
+      <c r="O24" s="10">
+        <f t="shared" si="0"/>
+        <v>-5.0971647694678168</v>
+      </c>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="10"/>
+      <c r="R24" s="16">
+        <v>47.603189912014201</v>
+      </c>
+      <c r="S24" s="6">
+        <f t="shared" si="1"/>
+        <v>-10.994375271524916</v>
+      </c>
+    </row>
+    <row r="25" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+      <c r="M25" s="5"/>
+      <c r="N25">
+        <v>63.268964480711197</v>
+      </c>
+      <c r="O25" s="10">
+        <f t="shared" si="0"/>
+        <v>4.6713992971720799</v>
+      </c>
+      <c r="P25" s="10"/>
+      <c r="Q25" s="10"/>
+      <c r="R25" s="16">
+        <v>63.999940981266398</v>
+      </c>
+      <c r="S25" s="6">
+        <f t="shared" si="1"/>
+        <v>5.4023757977272808</v>
+      </c>
+    </row>
+    <row r="26" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C26" t="s">
+        <v>12</v>
+      </c>
+      <c r="M26" s="5"/>
+      <c r="N26">
+        <v>54.885053067435898</v>
+      </c>
+      <c r="O26" s="10">
+        <f t="shared" si="0"/>
+        <v>-3.7125121161032197</v>
+      </c>
+      <c r="P26" s="10"/>
+      <c r="Q26" s="10"/>
+      <c r="R26" s="16">
+        <v>61.085403352154202</v>
+      </c>
+      <c r="S26" s="6">
+        <f t="shared" si="1"/>
+        <v>2.4878381686150846</v>
+      </c>
+    </row>
+    <row r="27" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="M27" s="5"/>
+      <c r="N27">
+        <v>51.391051951221797</v>
+      </c>
+      <c r="O27" s="10">
+        <f t="shared" si="0"/>
+        <v>-7.2065132323173202</v>
+      </c>
+      <c r="P27" s="10"/>
+      <c r="Q27" s="10"/>
+      <c r="R27" s="16">
+        <v>62.507350830789797</v>
+      </c>
+      <c r="S27" s="6">
+        <f t="shared" si="1"/>
+        <v>3.9097856472506791</v>
+      </c>
+    </row>
+    <row r="28" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="M28" s="5"/>
+      <c r="N28">
+        <v>55.077527171306699</v>
+      </c>
+      <c r="O28" s="10">
+        <f t="shared" si="0"/>
+        <v>-3.5200380122324191</v>
+      </c>
+      <c r="P28" s="10"/>
+      <c r="Q28" s="10"/>
+      <c r="R28" s="16">
+        <v>58.399858716019502</v>
+      </c>
+      <c r="S28" s="6">
+        <f t="shared" si="1"/>
+        <v>-0.19770646751961607</v>
+      </c>
+    </row>
+    <row r="29" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="M29" s="5"/>
+      <c r="N29">
+        <v>53.2855319311711</v>
+      </c>
+      <c r="O29" s="10">
+        <f t="shared" si="0"/>
+        <v>-5.3120332523680176</v>
+      </c>
+      <c r="P29" s="10"/>
+      <c r="Q29" s="10"/>
+      <c r="R29" s="16">
+        <v>62.902218073128203</v>
+      </c>
+      <c r="S29" s="6">
+        <f t="shared" si="1"/>
+        <v>4.3046528895890859</v>
+      </c>
+    </row>
+    <row r="30" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C30" t="s">
+        <v>8</v>
+      </c>
+      <c r="M30" s="5"/>
+      <c r="N30">
+        <v>51.206679765754103</v>
+      </c>
+      <c r="O30" s="10">
+        <f t="shared" si="0"/>
+        <v>-7.3908854177850145</v>
+      </c>
+      <c r="P30" s="10"/>
+      <c r="Q30" s="10"/>
+      <c r="R30" s="16">
+        <v>50.534387269948098</v>
+      </c>
+      <c r="S30" s="6">
+        <f t="shared" si="1"/>
+        <v>-8.0631779135910193</v>
+      </c>
+    </row>
+    <row r="31" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="M31" s="5"/>
+      <c r="N31">
+        <v>64.820412361810995</v>
+      </c>
+      <c r="O31" s="10">
+        <f t="shared" si="0"/>
+        <v>6.2228471782718771</v>
+      </c>
+      <c r="P31" s="10"/>
+      <c r="Q31" s="10"/>
+      <c r="R31" s="16">
+        <v>60.264646238055597</v>
+      </c>
+      <c r="S31" s="6">
+        <f t="shared" si="1"/>
+        <v>1.6670810545164798</v>
+      </c>
+    </row>
+    <row r="32" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="M32" s="5"/>
+      <c r="N32">
+        <v>59.317502533038798</v>
+      </c>
+      <c r="O32" s="10">
+        <f t="shared" si="0"/>
+        <v>0.71993734949968058</v>
+      </c>
+      <c r="P32" s="10"/>
+      <c r="Q32" s="10"/>
+      <c r="R32" s="16">
+        <v>56.207991064875202</v>
+      </c>
+      <c r="S32" s="6">
+        <f t="shared" si="1"/>
+        <v>-2.3895741186639157</v>
+      </c>
+    </row>
+    <row r="33" spans="3:34" x14ac:dyDescent="0.3">
+      <c r="M33" s="5"/>
+      <c r="N33">
+        <v>54.903918413070301</v>
+      </c>
+      <c r="O33" s="10">
+        <f t="shared" si="0"/>
+        <v>-3.693646770468817</v>
+      </c>
+      <c r="P33" s="10"/>
+      <c r="Q33" s="10"/>
+      <c r="R33" s="16">
+        <v>62.439512225719199</v>
+      </c>
+      <c r="S33" s="6">
+        <f>R33-N$2</f>
+        <v>3.841947042180081</v>
+      </c>
+    </row>
+    <row r="34" spans="3:34" x14ac:dyDescent="0.3">
+      <c r="M34" s="5"/>
+      <c r="N34">
+        <v>58.364709485529701</v>
+      </c>
+      <c r="O34" s="10">
+        <f t="shared" si="0"/>
+        <v>-0.2328556980094163</v>
+      </c>
+      <c r="P34" s="10"/>
+      <c r="Q34" s="10"/>
+      <c r="R34" s="16">
+        <v>66.447467634614995</v>
+      </c>
+      <c r="S34" s="6">
+        <f>R34-N$2</f>
+        <v>7.8499024510758773</v>
+      </c>
+    </row>
+    <row r="35" spans="3:34" x14ac:dyDescent="0.3">
+      <c r="M35" s="5"/>
+      <c r="N35">
+        <v>66.866787379290997</v>
+      </c>
+      <c r="O35" s="10">
+        <f t="shared" si="0"/>
+        <v>8.2692221957518797</v>
+      </c>
+      <c r="P35" s="10"/>
+      <c r="Q35" s="10"/>
+      <c r="R35" s="16">
+        <v>59.022839789896899</v>
+      </c>
+      <c r="S35" s="6">
+        <f>R35-N$2</f>
+        <v>0.42527460635778169</v>
+      </c>
+    </row>
+    <row r="36" spans="3:34" x14ac:dyDescent="0.3">
+      <c r="M36" s="5"/>
+      <c r="N36">
+        <v>59.388107079464199</v>
+      </c>
+      <c r="O36" s="10">
+        <f t="shared" si="0"/>
+        <v>0.79054189592508095</v>
+      </c>
+      <c r="P36" s="10"/>
+      <c r="Q36" s="10"/>
+      <c r="R36" s="16">
+        <v>57.561839131364998</v>
+      </c>
+      <c r="S36" s="6">
+        <f>R36-N$2</f>
+        <v>-1.0357260521741196</v>
+      </c>
+    </row>
+    <row r="37" spans="3:34" x14ac:dyDescent="0.3">
+      <c r="M37" s="5"/>
+      <c r="N37">
+        <v>53.551035496018699</v>
+      </c>
+      <c r="O37" s="10">
+        <f t="shared" si="0"/>
+        <v>-5.0465296875204189</v>
+      </c>
+      <c r="P37" s="10"/>
+      <c r="Q37" s="10"/>
+      <c r="R37" s="16">
+        <v>68.309327543851893</v>
+      </c>
+      <c r="S37" s="6">
+        <f>R37-N$2</f>
+        <v>9.7117623603127754</v>
+      </c>
+    </row>
+    <row r="38" spans="3:34" x14ac:dyDescent="0.3">
+      <c r="C38" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="M38" s="5"/>
+      <c r="N38">
+        <v>59.2199260218555</v>
+      </c>
+      <c r="O38" s="10">
+        <f t="shared" si="0"/>
+        <v>0.62236083831638211</v>
+      </c>
+      <c r="P38" s="10"/>
+      <c r="Q38" s="10"/>
+      <c r="R38" s="16">
+        <v>63.314556441683102</v>
+      </c>
+      <c r="S38" s="6">
+        <f>R38-N$2</f>
+        <v>4.7169912581439846</v>
+      </c>
+    </row>
+    <row r="39" spans="3:34" x14ac:dyDescent="0.3">
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="M39" s="5"/>
+      <c r="N39">
+        <v>60.5710064586928</v>
+      </c>
+      <c r="O39" s="10">
+        <f t="shared" si="0"/>
+        <v>1.9734412751536823</v>
+      </c>
+      <c r="P39" s="10"/>
+      <c r="Q39" s="10"/>
+      <c r="R39" s="16">
+        <v>58.977288895697399</v>
+      </c>
+      <c r="S39" s="6">
+        <f>R39-N$2</f>
+        <v>0.37972371215828105</v>
+      </c>
+    </row>
+    <row r="40" spans="3:34" x14ac:dyDescent="0.3">
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="M40" s="5"/>
+      <c r="N40">
+        <v>55.318585925233101</v>
+      </c>
+      <c r="O40" s="10">
+        <f t="shared" si="0"/>
+        <v>-3.2789792583060162</v>
+      </c>
+      <c r="P40" s="10"/>
+      <c r="Q40" s="10"/>
+      <c r="R40" s="16">
+        <v>52.478401637939101</v>
+      </c>
+      <c r="S40" s="6">
+        <f>R40-N$2</f>
+        <v>-6.1191635456000171</v>
+      </c>
+    </row>
+    <row r="41" spans="3:34" x14ac:dyDescent="0.3">
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="M41" s="5"/>
+      <c r="N41">
+        <v>62.905884149579201</v>
+      </c>
+      <c r="O41" s="10">
+        <f t="shared" si="0"/>
+        <v>4.3083189660400834</v>
+      </c>
+      <c r="P41" s="10"/>
+      <c r="Q41" s="10"/>
+      <c r="R41" s="16">
+        <v>52.1515765284704</v>
+      </c>
+      <c r="S41" s="6">
+        <f>R41-N$2</f>
+        <v>-6.4459886550687173</v>
+      </c>
+    </row>
+    <row r="42" spans="3:34" x14ac:dyDescent="0.3">
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="M42" s="5"/>
+      <c r="N42">
+        <v>58.137426962554997</v>
+      </c>
+      <c r="O42" s="10">
+        <f t="shared" si="0"/>
+        <v>-0.46013822098412049</v>
+      </c>
+      <c r="P42" s="10"/>
+      <c r="Q42" s="10"/>
+      <c r="R42" s="16">
+        <v>60.591040793208897</v>
+      </c>
+      <c r="S42" s="6">
+        <f>R42-N$2</f>
+        <v>1.9934756096697797</v>
+      </c>
+    </row>
+    <row r="43" spans="3:34" x14ac:dyDescent="0.3">
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="M43" s="5"/>
+      <c r="N43">
+        <v>54.811621685205701</v>
+      </c>
+      <c r="O43" s="10">
+        <f t="shared" si="0"/>
+        <v>-3.7859434983334168</v>
+      </c>
+      <c r="P43" s="10"/>
+      <c r="Q43" s="10"/>
+      <c r="R43" s="16">
+        <v>44.800829530442797</v>
+      </c>
+      <c r="S43" s="6">
+        <f>R43-N$2</f>
+        <v>-13.79673565309632</v>
+      </c>
+    </row>
+    <row r="44" spans="3:34" x14ac:dyDescent="0.3">
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="M44" s="5"/>
+      <c r="N44">
+        <v>55.350849773123699</v>
+      </c>
+      <c r="O44" s="10">
+        <f t="shared" si="0"/>
+        <v>-3.246715410415419</v>
+      </c>
+      <c r="P44" s="10"/>
+      <c r="Q44" s="10"/>
+      <c r="R44" s="16">
+        <v>52.361349076999197</v>
+      </c>
+      <c r="S44" s="6">
+        <f>R44-N$2</f>
+        <v>-6.2362161065399206</v>
+      </c>
+    </row>
+    <row r="45" spans="3:34" x14ac:dyDescent="0.3">
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="M45" s="5"/>
+      <c r="N45">
+        <v>51.628290765520298</v>
+      </c>
+      <c r="O45" s="10">
+        <f t="shared" si="0"/>
+        <v>-6.96927441801882</v>
+      </c>
+      <c r="P45" s="10"/>
+      <c r="Q45" s="10"/>
+      <c r="R45" s="16">
+        <v>66.4602014725982</v>
+      </c>
+      <c r="S45" s="6">
+        <f>R45-N$2</f>
+        <v>7.8626362890590826</v>
+      </c>
+    </row>
+    <row r="46" spans="3:34" x14ac:dyDescent="0.3">
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="M46" s="5"/>
+      <c r="N46">
+        <v>60.420619790768498</v>
+      </c>
+      <c r="O46" s="10">
+        <f t="shared" si="0"/>
+        <v>1.8230546072293805</v>
+      </c>
+      <c r="P46" s="10"/>
+      <c r="Q46" s="10"/>
+    </row>
+    <row r="47" spans="3:34" x14ac:dyDescent="0.3">
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+      <c r="M47" s="5"/>
+      <c r="N47">
+        <v>53.713421779336002</v>
+      </c>
+      <c r="O47" s="10">
+        <f t="shared" si="0"/>
+        <v>-4.8841434042031153</v>
+      </c>
+      <c r="P47" s="10"/>
+      <c r="Q47" s="10"/>
+      <c r="R47" s="10"/>
+      <c r="S47" s="6"/>
+    </row>
+    <row r="48" spans="3:34" x14ac:dyDescent="0.3">
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
+      <c r="M48" s="5"/>
+      <c r="N48" s="10"/>
+      <c r="O48" s="10"/>
+      <c r="P48" s="10"/>
+      <c r="Q48" s="10"/>
+      <c r="R48" s="10"/>
+      <c r="S48" s="6"/>
+      <c r="U48" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="V48" s="15"/>
+      <c r="W48" s="15"/>
+      <c r="X48" s="15"/>
+      <c r="Y48" s="15"/>
+      <c r="Z48" s="15"/>
+      <c r="AA48" s="15"/>
+      <c r="AB48" s="15"/>
+      <c r="AC48" s="15"/>
+      <c r="AD48" s="15"/>
+      <c r="AE48" s="15"/>
+      <c r="AF48" s="15"/>
+      <c r="AG48" s="15"/>
+      <c r="AH48" s="15"/>
+    </row>
+    <row r="49" spans="3:34" x14ac:dyDescent="0.3">
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
+      <c r="M49" s="5"/>
+      <c r="N49" s="10"/>
+      <c r="O49" s="10"/>
+      <c r="P49" s="10"/>
+      <c r="Q49" s="10"/>
+      <c r="R49" s="10"/>
+      <c r="S49" s="6"/>
+      <c r="U49" s="15"/>
+      <c r="V49" s="15"/>
+      <c r="W49" s="15"/>
+      <c r="X49" s="15"/>
+      <c r="Y49" s="15"/>
+      <c r="Z49" s="15"/>
+      <c r="AA49" s="15"/>
+      <c r="AB49" s="15"/>
+      <c r="AC49" s="15"/>
+      <c r="AD49" s="15"/>
+      <c r="AE49" s="15"/>
+      <c r="AF49" s="15"/>
+      <c r="AG49" s="15"/>
+      <c r="AH49" s="15"/>
+    </row>
+    <row r="50" spans="3:34" x14ac:dyDescent="0.3">
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
+      <c r="M50" s="5"/>
+      <c r="N50" s="10"/>
+      <c r="O50" s="10"/>
+      <c r="P50" s="10"/>
+      <c r="Q50" s="10"/>
+      <c r="R50" s="10"/>
+      <c r="S50" s="6"/>
+      <c r="U50" s="15"/>
+      <c r="V50" s="15"/>
+      <c r="W50" s="15"/>
+      <c r="X50" s="15"/>
+      <c r="Y50" s="15"/>
+      <c r="Z50" s="15"/>
+      <c r="AA50" s="15"/>
+      <c r="AB50" s="15"/>
+      <c r="AC50" s="15"/>
+      <c r="AD50" s="15"/>
+      <c r="AE50" s="15"/>
+      <c r="AF50" s="15"/>
+      <c r="AG50" s="15"/>
+      <c r="AH50" s="15"/>
+    </row>
+    <row r="51" spans="3:34" x14ac:dyDescent="0.3">
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="K51" s="2"/>
+      <c r="M51" s="5"/>
+      <c r="N51" s="10"/>
+      <c r="O51" s="10"/>
+      <c r="P51" s="10"/>
+      <c r="Q51" s="10"/>
+      <c r="R51" s="10"/>
+      <c r="S51" s="6"/>
+      <c r="U51" s="15"/>
+      <c r="V51" s="15"/>
+      <c r="W51" s="15"/>
+      <c r="X51" s="15"/>
+      <c r="Y51" s="15"/>
+      <c r="Z51" s="15"/>
+      <c r="AA51" s="15"/>
+      <c r="AB51" s="15"/>
+      <c r="AC51" s="15"/>
+      <c r="AD51" s="15"/>
+      <c r="AE51" s="15"/>
+      <c r="AF51" s="15"/>
+      <c r="AG51" s="15"/>
+      <c r="AH51" s="15"/>
+    </row>
+    <row r="52" spans="3:34" x14ac:dyDescent="0.3">
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+      <c r="K52" s="2"/>
+      <c r="M52" s="5"/>
+      <c r="N52" s="10"/>
+      <c r="O52" s="10"/>
+      <c r="P52" s="10"/>
+      <c r="Q52" s="10"/>
+      <c r="R52" s="10"/>
+      <c r="S52" s="6"/>
+      <c r="U52" s="15"/>
+      <c r="V52" s="15"/>
+      <c r="W52" s="15"/>
+      <c r="X52" s="15"/>
+      <c r="Y52" s="15"/>
+      <c r="Z52" s="15"/>
+      <c r="AA52" s="15"/>
+      <c r="AB52" s="15"/>
+      <c r="AC52" s="15"/>
+      <c r="AD52" s="15"/>
+      <c r="AE52" s="15"/>
+      <c r="AF52" s="15"/>
+      <c r="AG52" s="15"/>
+      <c r="AH52" s="15"/>
+    </row>
+    <row r="53" spans="3:34" x14ac:dyDescent="0.3">
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
+      <c r="J53" s="2"/>
+      <c r="K53" s="2"/>
+      <c r="M53" s="5"/>
+      <c r="N53" s="10"/>
+      <c r="O53" s="10"/>
+      <c r="P53" s="10"/>
+      <c r="Q53" s="10"/>
+      <c r="R53" s="10"/>
+      <c r="S53" s="6"/>
+      <c r="U53" s="15"/>
+      <c r="V53" s="15"/>
+      <c r="W53" s="15"/>
+      <c r="X53" s="15"/>
+      <c r="Y53" s="15"/>
+      <c r="Z53" s="15"/>
+      <c r="AA53" s="15"/>
+      <c r="AB53" s="15"/>
+      <c r="AC53" s="15"/>
+      <c r="AD53" s="15"/>
+      <c r="AE53" s="15"/>
+      <c r="AF53" s="15"/>
+      <c r="AG53" s="15"/>
+      <c r="AH53" s="15"/>
+    </row>
+    <row r="54" spans="3:34" x14ac:dyDescent="0.3">
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
+      <c r="I54" s="2"/>
+      <c r="J54" s="2"/>
+      <c r="K54" s="2"/>
+      <c r="M54" s="5"/>
+      <c r="N54" s="10"/>
+      <c r="O54" s="10"/>
+      <c r="P54" s="10"/>
+      <c r="Q54" s="10"/>
+      <c r="R54" s="10"/>
+      <c r="S54" s="6"/>
+      <c r="U54" s="15"/>
+      <c r="V54" s="15"/>
+      <c r="W54" s="15"/>
+      <c r="X54" s="15"/>
+      <c r="Y54" s="15"/>
+      <c r="Z54" s="15"/>
+      <c r="AA54" s="15"/>
+      <c r="AB54" s="15"/>
+      <c r="AC54" s="15"/>
+      <c r="AD54" s="15"/>
+      <c r="AE54" s="15"/>
+      <c r="AF54" s="15"/>
+      <c r="AG54" s="15"/>
+      <c r="AH54" s="15"/>
+    </row>
+    <row r="55" spans="3:34" x14ac:dyDescent="0.3">
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2"/>
+      <c r="H55" s="2"/>
+      <c r="I55" s="2"/>
+      <c r="J55" s="2"/>
+      <c r="K55" s="2"/>
+      <c r="M55" s="5"/>
+      <c r="N55" s="10"/>
+      <c r="O55" s="10"/>
+      <c r="P55" s="10"/>
+      <c r="Q55" s="10"/>
+      <c r="R55" s="10"/>
+      <c r="S55" s="6"/>
+      <c r="U55" s="15"/>
+      <c r="V55" s="15"/>
+      <c r="W55" s="15"/>
+      <c r="X55" s="15"/>
+      <c r="Y55" s="15"/>
+      <c r="Z55" s="15"/>
+      <c r="AA55" s="15"/>
+      <c r="AB55" s="15"/>
+      <c r="AC55" s="15"/>
+      <c r="AD55" s="15"/>
+      <c r="AE55" s="15"/>
+      <c r="AF55" s="15"/>
+      <c r="AG55" s="15"/>
+      <c r="AH55" s="15"/>
+    </row>
+    <row r="56" spans="3:34" x14ac:dyDescent="0.3">
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+      <c r="I56" s="2"/>
+      <c r="J56" s="2"/>
+      <c r="K56" s="2"/>
+      <c r="M56" s="5"/>
+      <c r="N56" s="10"/>
+      <c r="O56" s="10"/>
+      <c r="P56" s="10"/>
+      <c r="Q56" s="10"/>
+      <c r="R56" s="10"/>
+      <c r="S56" s="6"/>
+      <c r="U56" s="15"/>
+      <c r="V56" s="15"/>
+      <c r="W56" s="15"/>
+      <c r="X56" s="15"/>
+      <c r="Y56" s="15"/>
+      <c r="Z56" s="15"/>
+      <c r="AA56" s="15"/>
+      <c r="AB56" s="15"/>
+      <c r="AC56" s="15"/>
+      <c r="AD56" s="15"/>
+      <c r="AE56" s="15"/>
+      <c r="AF56" s="15"/>
+      <c r="AG56" s="15"/>
+      <c r="AH56" s="15"/>
+    </row>
+    <row r="57" spans="3:34" x14ac:dyDescent="0.3">
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2"/>
+      <c r="I57" s="2"/>
+      <c r="J57" s="2"/>
+      <c r="K57" s="2"/>
+      <c r="M57" s="5"/>
+      <c r="N57" s="10"/>
+      <c r="O57" s="10"/>
+      <c r="P57" s="10"/>
+      <c r="Q57" s="10"/>
+      <c r="R57" s="10"/>
+      <c r="S57" s="6"/>
+      <c r="U57" s="15"/>
+      <c r="V57" s="15"/>
+      <c r="W57" s="15"/>
+      <c r="X57" s="15"/>
+      <c r="Y57" s="15"/>
+      <c r="Z57" s="15"/>
+      <c r="AA57" s="15"/>
+      <c r="AB57" s="15"/>
+      <c r="AC57" s="15"/>
+      <c r="AD57" s="15"/>
+      <c r="AE57" s="15"/>
+      <c r="AF57" s="15"/>
+      <c r="AG57" s="15"/>
+      <c r="AH57" s="15"/>
+    </row>
+    <row r="58" spans="3:34" x14ac:dyDescent="0.3">
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+      <c r="G58" s="2"/>
+      <c r="H58" s="2"/>
+      <c r="I58" s="2"/>
+      <c r="J58" s="2"/>
+      <c r="K58" s="2"/>
+      <c r="M58" s="5"/>
+      <c r="N58" s="10"/>
+      <c r="O58" s="10"/>
+      <c r="P58" s="10"/>
+      <c r="Q58" s="10"/>
+      <c r="R58" s="10"/>
+      <c r="S58" s="6"/>
+      <c r="U58" s="15"/>
+      <c r="V58" s="15"/>
+      <c r="W58" s="15"/>
+      <c r="X58" s="15"/>
+      <c r="Y58" s="15"/>
+      <c r="Z58" s="15"/>
+      <c r="AA58" s="15"/>
+      <c r="AB58" s="15"/>
+      <c r="AC58" s="15"/>
+      <c r="AD58" s="15"/>
+      <c r="AE58" s="15"/>
+      <c r="AF58" s="15"/>
+      <c r="AG58" s="15"/>
+      <c r="AH58" s="15"/>
+    </row>
+    <row r="59" spans="3:34" x14ac:dyDescent="0.3">
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
+      <c r="G59" s="2"/>
+      <c r="H59" s="2"/>
+      <c r="I59" s="2"/>
+      <c r="J59" s="2"/>
+      <c r="K59" s="2"/>
+      <c r="M59" s="5"/>
+      <c r="N59" s="10"/>
+      <c r="O59" s="10"/>
+      <c r="P59" s="10"/>
+      <c r="Q59" s="10"/>
+      <c r="R59" s="10"/>
+      <c r="S59" s="6"/>
+      <c r="U59" s="15"/>
+      <c r="V59" s="15"/>
+      <c r="W59" s="15"/>
+      <c r="X59" s="15"/>
+      <c r="Y59" s="15"/>
+      <c r="Z59" s="15"/>
+      <c r="AA59" s="15"/>
+      <c r="AB59" s="15"/>
+      <c r="AC59" s="15"/>
+      <c r="AD59" s="15"/>
+      <c r="AE59" s="15"/>
+      <c r="AF59" s="15"/>
+      <c r="AG59" s="15"/>
+      <c r="AH59" s="15"/>
+    </row>
+    <row r="60" spans="3:34" x14ac:dyDescent="0.3">
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
+      <c r="F60" s="2"/>
+      <c r="G60" s="2"/>
+      <c r="H60" s="2"/>
+      <c r="I60" s="2"/>
+      <c r="J60" s="2"/>
+      <c r="K60" s="2"/>
+      <c r="M60" s="5"/>
+      <c r="N60" s="10"/>
+      <c r="O60" s="10"/>
+      <c r="P60" s="10"/>
+      <c r="Q60" s="10"/>
+      <c r="R60" s="10"/>
+      <c r="S60" s="6"/>
+      <c r="U60" s="15"/>
+      <c r="V60" s="15"/>
+      <c r="W60" s="15"/>
+      <c r="X60" s="15"/>
+      <c r="Y60" s="15"/>
+      <c r="Z60" s="15"/>
+      <c r="AA60" s="15"/>
+      <c r="AB60" s="15"/>
+      <c r="AC60" s="15"/>
+      <c r="AD60" s="15"/>
+      <c r="AE60" s="15"/>
+      <c r="AF60" s="15"/>
+      <c r="AG60" s="15"/>
+      <c r="AH60" s="15"/>
+    </row>
+    <row r="61" spans="3:34" x14ac:dyDescent="0.3">
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
+      <c r="G61" s="2"/>
+      <c r="H61" s="2"/>
+      <c r="I61" s="2"/>
+      <c r="J61" s="2"/>
+      <c r="K61" s="2"/>
+      <c r="M61" s="5"/>
+      <c r="N61" s="10"/>
+      <c r="O61" s="10"/>
+      <c r="P61" s="10"/>
+      <c r="Q61" s="10"/>
+      <c r="R61" s="10"/>
+      <c r="S61" s="6"/>
+      <c r="U61" s="15"/>
+      <c r="V61" s="15"/>
+      <c r="W61" s="15"/>
+      <c r="X61" s="15"/>
+      <c r="Y61" s="15"/>
+      <c r="Z61" s="15"/>
+      <c r="AA61" s="15"/>
+      <c r="AB61" s="15"/>
+      <c r="AC61" s="15"/>
+      <c r="AD61" s="15"/>
+      <c r="AE61" s="15"/>
+      <c r="AF61" s="15"/>
+      <c r="AG61" s="15"/>
+      <c r="AH61" s="15"/>
+    </row>
+    <row r="62" spans="3:34" x14ac:dyDescent="0.3">
+      <c r="M62" s="5"/>
+      <c r="N62" s="10"/>
+      <c r="O62" s="10"/>
+      <c r="P62" s="10"/>
+      <c r="Q62" s="10"/>
+      <c r="R62" s="10"/>
+      <c r="S62" s="6"/>
+      <c r="U62" s="15"/>
+      <c r="V62" s="15"/>
+      <c r="W62" s="15"/>
+      <c r="X62" s="15"/>
+      <c r="Y62" s="15"/>
+      <c r="Z62" s="15"/>
+      <c r="AA62" s="15"/>
+      <c r="AB62" s="15"/>
+      <c r="AC62" s="15"/>
+      <c r="AD62" s="15"/>
+      <c r="AE62" s="15"/>
+      <c r="AF62" s="15"/>
+      <c r="AG62" s="15"/>
+      <c r="AH62" s="15"/>
+    </row>
+    <row r="63" spans="3:34" x14ac:dyDescent="0.3">
+      <c r="M63" s="5"/>
+      <c r="N63" s="10"/>
+      <c r="O63" s="10"/>
+      <c r="P63" s="10"/>
+      <c r="Q63" s="10"/>
+      <c r="R63" s="10"/>
+      <c r="S63" s="6"/>
+      <c r="U63" s="15"/>
+      <c r="V63" s="15"/>
+      <c r="W63" s="15"/>
+      <c r="X63" s="15"/>
+      <c r="Y63" s="15"/>
+      <c r="Z63" s="15"/>
+      <c r="AA63" s="15"/>
+      <c r="AB63" s="15"/>
+      <c r="AC63" s="15"/>
+      <c r="AD63" s="15"/>
+      <c r="AE63" s="15"/>
+      <c r="AF63" s="15"/>
+      <c r="AG63" s="15"/>
+      <c r="AH63" s="15"/>
+    </row>
+    <row r="64" spans="3:34" x14ac:dyDescent="0.3">
+      <c r="M64" s="5"/>
+      <c r="N64" s="10"/>
+      <c r="O64" s="10"/>
+      <c r="P64" s="10"/>
+      <c r="Q64" s="10"/>
+      <c r="R64" s="10"/>
+      <c r="S64" s="6"/>
+      <c r="U64" s="15"/>
+      <c r="V64" s="15"/>
+      <c r="W64" s="15"/>
+      <c r="X64" s="15"/>
+      <c r="Y64" s="15"/>
+      <c r="Z64" s="15"/>
+      <c r="AA64" s="15"/>
+      <c r="AB64" s="15"/>
+      <c r="AC64" s="15"/>
+      <c r="AD64" s="15"/>
+      <c r="AE64" s="15"/>
+      <c r="AF64" s="15"/>
+      <c r="AG64" s="15"/>
+      <c r="AH64" s="15"/>
+    </row>
+    <row r="65" spans="13:34" x14ac:dyDescent="0.3">
+      <c r="M65" s="5"/>
+      <c r="N65" s="10"/>
+      <c r="O65" s="10"/>
+      <c r="P65" s="10"/>
+      <c r="Q65" s="10"/>
+      <c r="R65" s="10"/>
+      <c r="S65" s="6"/>
+      <c r="U65" s="15"/>
+      <c r="V65" s="15"/>
+      <c r="W65" s="15"/>
+      <c r="X65" s="15"/>
+      <c r="Y65" s="15"/>
+      <c r="Z65" s="15"/>
+      <c r="AA65" s="15"/>
+      <c r="AB65" s="15"/>
+      <c r="AC65" s="15"/>
+      <c r="AD65" s="15"/>
+      <c r="AE65" s="15"/>
+      <c r="AF65" s="15"/>
+      <c r="AG65" s="15"/>
+      <c r="AH65" s="15"/>
+    </row>
+    <row r="66" spans="13:34" x14ac:dyDescent="0.3">
+      <c r="M66" s="5"/>
+      <c r="N66" s="10"/>
+      <c r="O66" s="10"/>
+      <c r="P66" s="10"/>
+      <c r="Q66" s="10"/>
+      <c r="R66" s="10"/>
+      <c r="S66" s="6"/>
+      <c r="U66" s="15"/>
+      <c r="V66" s="15"/>
+      <c r="W66" s="15"/>
+      <c r="X66" s="15"/>
+      <c r="Y66" s="15"/>
+      <c r="Z66" s="15"/>
+      <c r="AA66" s="15"/>
+      <c r="AB66" s="15"/>
+      <c r="AC66" s="15"/>
+      <c r="AD66" s="15"/>
+      <c r="AE66" s="15"/>
+      <c r="AF66" s="15"/>
+      <c r="AG66" s="15"/>
+      <c r="AH66" s="15"/>
+    </row>
+    <row r="67" spans="13:34" x14ac:dyDescent="0.3">
+      <c r="M67" s="5"/>
+      <c r="N67" s="10"/>
+      <c r="O67" s="10"/>
+      <c r="P67" s="10"/>
+      <c r="Q67" s="10"/>
+      <c r="R67" s="10"/>
+      <c r="S67" s="6"/>
+      <c r="U67" s="15"/>
+      <c r="V67" s="15"/>
+      <c r="W67" s="15"/>
+      <c r="X67" s="15"/>
+      <c r="Y67" s="15"/>
+      <c r="Z67" s="15"/>
+      <c r="AA67" s="15"/>
+      <c r="AB67" s="15"/>
+      <c r="AC67" s="15"/>
+      <c r="AD67" s="15"/>
+      <c r="AE67" s="15"/>
+      <c r="AF67" s="15"/>
+      <c r="AG67" s="15"/>
+      <c r="AH67" s="15"/>
+    </row>
+    <row r="68" spans="13:34" x14ac:dyDescent="0.3">
+      <c r="M68" s="5"/>
+      <c r="N68" s="10"/>
+      <c r="O68" s="10"/>
+      <c r="P68" s="10"/>
+      <c r="Q68" s="10"/>
+      <c r="R68" s="10"/>
+      <c r="S68" s="6"/>
+      <c r="U68" s="15"/>
+      <c r="V68" s="15"/>
+      <c r="W68" s="15"/>
+      <c r="X68" s="15"/>
+      <c r="Y68" s="15"/>
+      <c r="Z68" s="15"/>
+      <c r="AA68" s="15"/>
+      <c r="AB68" s="15"/>
+      <c r="AC68" s="15"/>
+      <c r="AD68" s="15"/>
+      <c r="AE68" s="15"/>
+      <c r="AF68" s="15"/>
+      <c r="AG68" s="15"/>
+      <c r="AH68" s="15"/>
+    </row>
+    <row r="69" spans="13:34" x14ac:dyDescent="0.3">
+      <c r="M69" s="5"/>
+      <c r="N69" s="10"/>
+      <c r="O69" s="10"/>
+      <c r="P69" s="10"/>
+      <c r="Q69" s="10"/>
+      <c r="R69" s="10"/>
+      <c r="S69" s="6"/>
+      <c r="U69" s="15"/>
+      <c r="V69" s="15"/>
+      <c r="W69" s="15"/>
+      <c r="X69" s="15"/>
+      <c r="Y69" s="15"/>
+      <c r="Z69" s="15"/>
+      <c r="AA69" s="15"/>
+      <c r="AB69" s="15"/>
+      <c r="AC69" s="15"/>
+      <c r="AD69" s="15"/>
+      <c r="AE69" s="15"/>
+      <c r="AF69" s="15"/>
+      <c r="AG69" s="15"/>
+      <c r="AH69" s="15"/>
+    </row>
+    <row r="70" spans="13:34" x14ac:dyDescent="0.3">
+      <c r="M70" s="5"/>
+      <c r="N70" s="10"/>
+      <c r="O70" s="10"/>
+      <c r="P70" s="10"/>
+      <c r="Q70" s="10"/>
+      <c r="R70" s="10"/>
+      <c r="S70" s="6"/>
+      <c r="U70" s="15"/>
+      <c r="V70" s="15"/>
+      <c r="W70" s="15"/>
+      <c r="X70" s="15"/>
+      <c r="Y70" s="15"/>
+      <c r="Z70" s="15"/>
+      <c r="AA70" s="15"/>
+      <c r="AB70" s="15"/>
+      <c r="AC70" s="15"/>
+      <c r="AD70" s="15"/>
+      <c r="AE70" s="15"/>
+      <c r="AF70" s="15"/>
+      <c r="AG70" s="15"/>
+      <c r="AH70" s="15"/>
+    </row>
+    <row r="71" spans="13:34" x14ac:dyDescent="0.3">
+      <c r="M71" s="7"/>
+      <c r="N71" s="11"/>
+      <c r="O71" s="11"/>
+      <c r="P71" s="11"/>
+      <c r="Q71" s="11"/>
+      <c r="R71" s="11"/>
+      <c r="S71" s="8"/>
+      <c r="U71" s="15"/>
+      <c r="V71" s="15"/>
+      <c r="W71" s="15"/>
+      <c r="X71" s="15"/>
+      <c r="Y71" s="15"/>
+      <c r="Z71" s="15"/>
+      <c r="AA71" s="15"/>
+      <c r="AB71" s="15"/>
+      <c r="AC71" s="15"/>
+      <c r="AD71" s="15"/>
+      <c r="AE71" s="15"/>
+      <c r="AF71" s="15"/>
+      <c r="AG71" s="15"/>
+      <c r="AH71" s="15"/>
+    </row>
+    <row r="72" spans="13:34" x14ac:dyDescent="0.3">
+      <c r="U72" s="15"/>
+      <c r="V72" s="15"/>
+      <c r="W72" s="15"/>
+      <c r="X72" s="15"/>
+      <c r="Y72" s="15"/>
+      <c r="Z72" s="15"/>
+      <c r="AA72" s="15"/>
+      <c r="AB72" s="15"/>
+      <c r="AC72" s="15"/>
+      <c r="AD72" s="15"/>
+      <c r="AE72" s="15"/>
+      <c r="AF72" s="15"/>
+      <c r="AG72" s="15"/>
+      <c r="AH72" s="15"/>
+    </row>
+    <row r="73" spans="13:34" x14ac:dyDescent="0.3">
+      <c r="U73" s="15"/>
+      <c r="V73" s="15"/>
+      <c r="W73" s="15"/>
+      <c r="X73" s="15"/>
+      <c r="Y73" s="15"/>
+      <c r="Z73" s="15"/>
+      <c r="AA73" s="15"/>
+      <c r="AB73" s="15"/>
+      <c r="AC73" s="15"/>
+      <c r="AD73" s="15"/>
+      <c r="AE73" s="15"/>
+      <c r="AF73" s="15"/>
+      <c r="AG73" s="15"/>
+      <c r="AH73" s="15"/>
+    </row>
+    <row r="74" spans="13:34" x14ac:dyDescent="0.3">
+      <c r="U74" s="15"/>
+      <c r="V74" s="15"/>
+      <c r="W74" s="15"/>
+      <c r="X74" s="15"/>
+      <c r="Y74" s="15"/>
+      <c r="Z74" s="15"/>
+      <c r="AA74" s="15"/>
+      <c r="AB74" s="15"/>
+      <c r="AC74" s="15"/>
+      <c r="AD74" s="15"/>
+      <c r="AE74" s="15"/>
+      <c r="AF74" s="15"/>
+      <c r="AG74" s="15"/>
+      <c r="AH74" s="15"/>
+    </row>
+    <row r="75" spans="13:34" x14ac:dyDescent="0.3">
+      <c r="U75" s="15"/>
+      <c r="V75" s="15"/>
+      <c r="W75" s="15"/>
+      <c r="X75" s="15"/>
+      <c r="Y75" s="15"/>
+      <c r="Z75" s="15"/>
+      <c r="AA75" s="15"/>
+      <c r="AB75" s="15"/>
+      <c r="AC75" s="15"/>
+      <c r="AD75" s="15"/>
+      <c r="AE75" s="15"/>
+      <c r="AF75" s="15"/>
+      <c r="AG75" s="15"/>
+      <c r="AH75" s="15"/>
+    </row>
+    <row r="76" spans="13:34" x14ac:dyDescent="0.3">
+      <c r="U76" s="15"/>
+      <c r="V76" s="15"/>
+      <c r="W76" s="15"/>
+      <c r="X76" s="15"/>
+      <c r="Y76" s="15"/>
+      <c r="Z76" s="15"/>
+      <c r="AA76" s="15"/>
+      <c r="AB76" s="15"/>
+      <c r="AC76" s="15"/>
+      <c r="AD76" s="15"/>
+      <c r="AE76" s="15"/>
+      <c r="AF76" s="15"/>
+      <c r="AG76" s="15"/>
+      <c r="AH76" s="15"/>
+    </row>
+    <row r="77" spans="13:34" x14ac:dyDescent="0.3">
+      <c r="U77" s="15"/>
+      <c r="V77" s="15"/>
+      <c r="W77" s="15"/>
+      <c r="X77" s="15"/>
+      <c r="Y77" s="15"/>
+      <c r="Z77" s="15"/>
+      <c r="AA77" s="15"/>
+      <c r="AB77" s="15"/>
+      <c r="AC77" s="15"/>
+      <c r="AD77" s="15"/>
+      <c r="AE77" s="15"/>
+      <c r="AF77" s="15"/>
+      <c r="AG77" s="15"/>
+      <c r="AH77" s="15"/>
+    </row>
+    <row r="78" spans="13:34" x14ac:dyDescent="0.3">
+      <c r="U78" s="15"/>
+      <c r="V78" s="15"/>
+      <c r="W78" s="15"/>
+      <c r="X78" s="15"/>
+      <c r="Y78" s="15"/>
+      <c r="Z78" s="15"/>
+      <c r="AA78" s="15"/>
+      <c r="AB78" s="15"/>
+      <c r="AC78" s="15"/>
+      <c r="AD78" s="15"/>
+      <c r="AE78" s="15"/>
+      <c r="AF78" s="15"/>
+      <c r="AG78" s="15"/>
+      <c r="AH78" s="15"/>
+    </row>
+    <row r="79" spans="13:34" x14ac:dyDescent="0.3">
+      <c r="U79" s="15"/>
+      <c r="V79" s="15"/>
+      <c r="W79" s="15"/>
+      <c r="X79" s="15"/>
+      <c r="Y79" s="15"/>
+      <c r="Z79" s="15"/>
+      <c r="AA79" s="15"/>
+      <c r="AB79" s="15"/>
+      <c r="AC79" s="15"/>
+      <c r="AD79" s="15"/>
+      <c r="AE79" s="15"/>
+      <c r="AF79" s="15"/>
+      <c r="AG79" s="15"/>
+      <c r="AH79" s="15"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="N18:N35">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R18:R45">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N18:N67">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R18:R44">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ADBA590-9498-4BDD-A1D6-7F20FBE88CCD}">
+  <dimension ref="A1:D29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>66.614839512964096</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>50.387895973150002</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <f>AVERAGE(A1:A29)</f>
+        <v>62.624590419121944</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>55.240574533909097</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>49.062274564435</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>75.343739535533501</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>54.272874134086301</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>55.290686805701498</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>83.847086855025296</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>51.032611690966903</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>56.163429958565501</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>53.8861919669069</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>52.4676277091922</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>84.185290159499303</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>53.425673631414497</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>57.205284240572098</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>91.385994678641197</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>54.442761657870001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>54.485592296231601</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>76.539122821437203</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>55.896076398212898</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>49.4527527587938</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>61.383140908175697</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>63.134707261721303</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>71.181231717212597</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>87.219581061164206</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>64.512049976052396</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>59.253744868826502</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>62.033701929497902</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>66.766582548776697</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>